<commit_message>
Gen1 and Gen2 with same features
</commit_message>
<xml_diff>
--- a/example/vpc-gen2.xlsx
+++ b/example/vpc-gen2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/gen2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE48E137-EB72-5643-9731-1ADB19B7EA54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A38F8F7-7125-D84A-832A-296B23299422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37720" yWindow="-20280" windowWidth="38400" windowHeight="20280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vpc" sheetId="6" r:id="rId1"/>
@@ -301,9 +301,6 @@
     <t>*group_name</t>
   </si>
   <si>
-    <t>vsi1nic1:subnet2:sg2:fip2;vsi1nic2:subnet3:sg1</t>
-  </si>
-  <si>
     <t>Ubuntu Linux 16.04 LTS - Minimal Install</t>
   </si>
   <si>
@@ -311,6 +308,9 @@
   </si>
   <si>
     <t>vsi4</t>
+  </si>
+  <si>
+    <t>vsi1nic1:subnet2:sg1:fip2;vsi1nic2:subnet2:sg2</t>
   </si>
   <si>
     <t>vpc1</t>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1924,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>35</v>
@@ -1958,7 +1958,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>74</v>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>35</v>
@@ -2184,7 +2184,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A27DA9FB-C6DE-DD43-83A1-C14B1BF5FE4D}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2218,7 +2220,7 @@
         <v>60</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
         <v>56</v>
@@ -2232,7 +2234,7 @@
         <v>61</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
         <v>57</v>
@@ -2243,10 +2245,10 @@
         <v>36</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
         <v>58</v>
@@ -2257,7 +2259,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
         <v>59</v>
@@ -2265,62 +2267,62 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E6" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E7" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E8" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E9" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E10" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E11" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E12" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E13" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E14" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E15" s="11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E16" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="11" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>